<commit_message>
Caja Negra y Planteamiento v2
</commit_message>
<xml_diff>
--- a/src/Caja Negra Teclado.xlsx
+++ b/src/Caja Negra Teclado.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="90">
   <si>
     <t>Clases de equivalencia no válidas</t>
   </si>
@@ -177,21 +177,9 @@
     <t>-32,768, 32,767</t>
   </si>
   <si>
-    <t>Límites Double</t>
-  </si>
-  <si>
-    <t>Límites Float</t>
-  </si>
-  <si>
     <t>-9,223,372,036,854,775,808,  9,223,372,036,854,775,807</t>
   </si>
   <si>
-    <t>1 (true) , 2 (false)</t>
-  </si>
-  <si>
-    <t>''s' || 'S' (true) , 'n' || 'N' (false)</t>
-  </si>
-  <si>
     <t>Leer Booleano (S o N)</t>
   </si>
   <si>
@@ -237,54 +225,15 @@
     <t>Rangos.MININMAXEX (num = 3,5, min=0, max=10)</t>
   </si>
   <si>
-    <t>2, infinito || -infinito, 1</t>
-  </si>
-  <si>
     <t>Leer Booleano (s o n)</t>
   </si>
   <si>
-    <t>Todos los caracteres menos 's', 'S', 'n', y 'N'</t>
-  </si>
-  <si>
-    <t>Todos los números decimales menos los comprendidos entre los límites Double</t>
-  </si>
-  <si>
-    <t>-infinito, -2,147,483,649 || 2,147,483,648, infinito (enteros)</t>
-  </si>
-  <si>
-    <t>Todos los números decimales menos los comprendidos entre los límites Float</t>
-  </si>
-  <si>
-    <t>-infinito, -32,769 || 32,768, infinito (enteros)</t>
-  </si>
-  <si>
-    <t>-infinito, -129 || 128, infinito (enteros)</t>
-  </si>
-  <si>
-    <t>-infinito, -9,223,372,036,854,775,809 ||  9,223,372,036,854,775,808, infinito (enteros)</t>
-  </si>
-  <si>
     <t>Leer numero entre un rango</t>
   </si>
   <si>
     <t>max &gt; min</t>
   </si>
   <si>
-    <t>min &lt;= max (7 &lt;= 7)</t>
-  </si>
-  <si>
-    <t>num &gt;= x (3 &gt;= 3)</t>
-  </si>
-  <si>
-    <t>num &lt;= x (3 &lt;= 3)</t>
-  </si>
-  <si>
-    <t>num &gt; x (3.1 &gt; 3)</t>
-  </si>
-  <si>
-    <t>null , \uffff</t>
-  </si>
-  <si>
     <t>Equivalencias.MAYORIGUAL (3&gt;=1 || 4.2 &gt;= 0 || 9&gt;=9)</t>
   </si>
   <si>
@@ -297,7 +246,49 @@
     <t>Equivalencias.MAYOR (3&gt;1 || 4 &gt; 0)</t>
   </si>
   <si>
-    <t>num &lt; x (-2 &lt; -2,1)</t>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Rango Double</t>
+  </si>
+  <si>
+    <t>Rango Float</t>
+  </si>
+  <si>
+    <t>x, num (num &lt; x)</t>
+  </si>
+  <si>
+    <t>x, num (num &gt; x)</t>
+  </si>
+  <si>
+    <t>num, x (num &lt;= x)</t>
+  </si>
+  <si>
+    <t>num, x (num &gt;= x)</t>
+  </si>
+  <si>
+    <t>min, max (min &lt;= max)</t>
+  </si>
+  <si>
+    <t>3, infinito || -infinito, 0</t>
+  </si>
+  <si>
+    <t>-infinito, -2,147,483,649 || 2,147,483,648, infinito</t>
+  </si>
+  <si>
+    <t>Fuera Rango Double</t>
+  </si>
+  <si>
+    <t>Fuera Rango Float</t>
+  </si>
+  <si>
+    <t>-infinito, -32,769 || 32,768, infinito</t>
+  </si>
+  <si>
+    <t>-infinito, -129 || 128, infinito</t>
+  </si>
+  <si>
+    <t>-infinito, -9,223,372,036,854,775,809 ||  9,223,372,036,854,775,808, infinito</t>
   </si>
 </sst>
 </file>
@@ -701,7 +692,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -745,6 +736,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -754,9 +763,6 @@
     <xf numFmtId="0" fontId="16" fillId="15" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,16 +775,13 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1086,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ36"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="AH18" sqref="AH18"/>
+    <sheetView tabSelected="1" topLeftCell="AG25" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1114,158 +1117,161 @@
     <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="17.375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="53.875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="70.625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33.75" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.625" customWidth="1"/>
+    <col min="33" max="33" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="53.875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="70.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="16" t="s">
+    <row r="1" spans="1:37" ht="14.25" customHeight="1">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="15" t="s">
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AI1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AJ1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AK1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-    </row>
-    <row r="3" spans="1:36" ht="14.25" customHeight="1">
+    <row r="2" spans="1:37" ht="14.25" customHeight="1">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="21"/>
+    </row>
+    <row r="3" spans="1:37" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
+      <c r="K3" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
       <c r="T3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="U3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="X3" s="18"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" s="20"/>
       <c r="Y3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1287,55 +1293,56 @@
       <c r="AE3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
-    </row>
-    <row r="4" spans="1:36" ht="14.25" customHeight="1">
+      <c r="AF3" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="21"/>
+    </row>
+    <row r="4" spans="1:37" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="26"/>
+      <c r="P4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="Q4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="R4" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>18</v>
@@ -1374,443 +1381,442 @@
         <v>29</v>
       </c>
       <c r="AF4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-    </row>
-    <row r="5" spans="1:36" ht="15">
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="21"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
+    </row>
+    <row r="5" spans="1:37" ht="15">
       <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG5" s="12" t="s">
+      <c r="AH5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AH5" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI5" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" ht="15">
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="15">
       <c r="B6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG6" s="6" t="s">
+      <c r="AH6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" ht="15">
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="15">
       <c r="C7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG7" s="6" t="s">
+      <c r="AH7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AH7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI7" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" ht="15">
+      <c r="AI7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ7" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="15">
       <c r="D8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG8" s="13" t="s">
+      <c r="AH8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AH8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI8" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" ht="15">
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="15">
       <c r="E9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG9" s="1" t="s">
+      <c r="AH9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AH9" s="13" t="s">
+      <c r="AI9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AI9" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" ht="15">
+      <c r="AJ9" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="15">
       <c r="F10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG10" s="1" t="s">
+      <c r="AH10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AH10" s="13" t="s">
+      <c r="AI10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AI10" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" ht="15">
+      <c r="AJ10" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" ht="15">
       <c r="G11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AH11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AH11" s="13" t="s">
+      <c r="AI11" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AI11" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" ht="15">
+      <c r="AJ11" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" ht="15">
       <c r="H12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG12" s="13" t="s">
+      <c r="AH12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AH12" s="1" t="s">
+      <c r="AI12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ12" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" ht="15">
+      <c r="I13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" ht="15">
+      <c r="J14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="AI12" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" ht="15">
-      <c r="I13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG13" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI13" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" ht="15">
-      <c r="J14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH14" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI14" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" ht="15">
+      <c r="AJ14" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="15">
       <c r="K15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG15" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="AH15" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI15" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" ht="15">
+        <v>71</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ15" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" ht="15">
       <c r="L16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH16" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI16" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="13:35" ht="15">
+      <c r="AH16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ16" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="13:36" ht="15">
       <c r="M17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH17" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI17" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="13:35" ht="15">
+      <c r="AH17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI17" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ17" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="13:36" ht="15">
       <c r="N18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH18" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI18" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="13:35" ht="15">
+      <c r="AH18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ18" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="13:36" ht="15">
       <c r="P19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH19" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI19" s="24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="13:35" ht="15">
+      <c r="AH19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI19" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ19" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="13:36" ht="15">
       <c r="Q20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH20" s="23"/>
-      <c r="AI20" s="24"/>
-    </row>
-    <row r="21" spans="13:35" ht="15">
+      <c r="AH20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI20" s="16"/>
+      <c r="AJ20" s="17"/>
+    </row>
+    <row r="21" spans="13:36" ht="15">
       <c r="R21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH21" s="23"/>
-      <c r="AI21" s="24"/>
-    </row>
-    <row r="22" spans="13:35" ht="15">
+      <c r="AH21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI21" s="16"/>
+      <c r="AJ21" s="17"/>
+    </row>
+    <row r="22" spans="13:36" ht="15">
       <c r="S22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH22" s="23"/>
-      <c r="AI22" s="24"/>
-    </row>
-    <row r="23" spans="13:35" ht="15">
+      <c r="AH22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI22" s="16"/>
+      <c r="AJ22" s="17"/>
+    </row>
+    <row r="23" spans="13:36" ht="15">
       <c r="T23" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="AG23" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="AH23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AI23" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="13:35" ht="15">
+      <c r="AI23" s="13"/>
+      <c r="AJ23" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="13:36" ht="15">
       <c r="U24" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG24" s="1" t="s">
+      <c r="AH24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI24" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="13:35" ht="15">
+      <c r="AI24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ24" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="13:36" ht="15">
       <c r="V25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG25" s="1" t="s">
+      <c r="AH25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AH25" s="1"/>
-      <c r="AI25" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="13:35" ht="15">
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="13:36" ht="15">
       <c r="W26" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG26" s="13" t="s">
+      <c r="AH26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AH26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI26" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="13:35" ht="15">
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="13:36" ht="15">
       <c r="X27" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="AG27" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="AH27" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AI27" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="13:35" ht="15">
+      <c r="AI27" s="13"/>
+      <c r="AJ27" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="13:36" ht="15">
       <c r="Y28" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG28" s="13" t="s">
+      <c r="AH28" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AH28" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI28" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="13:35" ht="15">
+      <c r="AI28" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ28" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="13:36" ht="15">
       <c r="Z29" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG29" s="1" t="s">
+      <c r="AH29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AH29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI29" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="13:35" ht="15">
+      <c r="AI29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ29" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="13:36" ht="15">
       <c r="AA30" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG30" s="1" t="s">
+      <c r="AH30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AH30" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI30" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="13:35" ht="15">
+      <c r="AI30" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ30" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="13:36" ht="15">
       <c r="AB31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG31" s="1" t="s">
+      <c r="AH31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AH31" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI31" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="13:35" ht="15">
+      <c r="AI31" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ31" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="13:36" ht="15">
       <c r="AC32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG32" s="1" t="s">
+      <c r="AH32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AH32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI32" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="30:35" ht="15">
+      <c r="AI32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ32" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="30:36" ht="15">
       <c r="AD33" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG33" s="1" t="s">
+      <c r="AH33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AH33" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI33" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="30:35" ht="15">
+      <c r="AI33" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ33" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="30:36" ht="15">
       <c r="AE34" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG34" s="1" t="s">
+      <c r="AF34" s="28"/>
+      <c r="AH34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AH34" s="1"/>
-      <c r="AI34" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="30:35" ht="15">
-      <c r="AF35" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG35" s="1" t="s">
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="30:36" ht="15">
+      <c r="AE35" s="28"/>
+      <c r="AF35" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH35" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI35" s="14"/>
+      <c r="AJ35" s="15"/>
+    </row>
+    <row r="36" spans="30:36" ht="15">
+      <c r="AG36" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AH35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI35" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="30:35">
-      <c r="AH36" s="1"/>
+      <c r="AI36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ36" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="30:36">
+      <c r="AI37" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="AH19:AH22"/>
-    <mergeCell ref="AI19:AI22"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="E3:E4"/>
+  <mergeCells count="21">
+    <mergeCell ref="AK1:AK4"/>
+    <mergeCell ref="T1:AG2"/>
     <mergeCell ref="AH1:AH4"/>
-    <mergeCell ref="AI1:AI4"/>
-    <mergeCell ref="AJ1:AJ4"/>
-    <mergeCell ref="T1:AF2"/>
-    <mergeCell ref="AG1:AG4"/>
     <mergeCell ref="P3:S3"/>
     <mergeCell ref="A1:S2"/>
     <mergeCell ref="U3:V3"/>
@@ -1822,6 +1828,13 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AI19:AI22"/>
+    <mergeCell ref="AJ19:AJ22"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="AI1:AI4"/>
+    <mergeCell ref="AJ1:AJ4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157505" bottom="0.39370078740157505" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
String no puede ser vacio
</commit_message>
<xml_diff>
--- a/src/Caja Negra Teclado.xlsx
+++ b/src/Caja Negra Teclado.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="93">
   <si>
     <t>Clases de equivalencia no válidas</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>-infinito, -9,223,372,036,854,775,809 ||  9,223,372,036,854,775,808, infinito</t>
+  </si>
+  <si>
+    <t>Leer String</t>
+  </si>
+  <si>
+    <t>Cadena vacia</t>
+  </si>
+  <si>
+    <t>""</t>
   </si>
 </sst>
 </file>
@@ -415,7 +424,7 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +518,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9BBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,7 +713,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -745,43 +766,58 @@
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="11" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1089,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK37"/>
+  <dimension ref="A1:AL38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG25" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="AH35" sqref="AH35"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1:AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1106,30 +1142,31 @@
     <col min="17" max="17" width="33" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="38.875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="38" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.125" customWidth="1"/>
-    <col min="25" max="25" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.625" customWidth="1"/>
-    <col min="33" max="33" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="53.875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="70.625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="33.75" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="38" customWidth="1"/>
+    <col min="21" max="21" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.125" customWidth="1"/>
+    <col min="26" max="26" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.625" customWidth="1"/>
+    <col min="34" max="34" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="53.875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="70.625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="14.25" customHeight="1">
+    <row r="1" spans="1:38" ht="14.25" customHeight="1">
       <c r="A1" s="24"/>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1149,36 +1186,37 @@
       <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
       <c r="S1" s="24"/>
-      <c r="T1" s="22" t="s">
+      <c r="T1" s="35"/>
+      <c r="U1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="21" t="s">
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="AI1" s="21" t="s">
+      <c r="AJ1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AK1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AL1" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="14.25" customHeight="1">
+    <row r="2" spans="1:38" ht="14.25" customHeight="1">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1198,30 +1236,31 @@
       <c r="Q2" s="24"/>
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-    </row>
-    <row r="3" spans="1:37" ht="14.25" customHeight="1">
+      <c r="T2" s="35"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+    </row>
+    <row r="3" spans="1:38" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="32" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1230,22 +1269,22 @@
       <c r="D3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="23" t="s">
         <v>16</v>
       </c>
       <c r="K3" s="25" t="s">
@@ -1255,70 +1294,73 @@
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="25"/>
-      <c r="P3" s="20" t="s">
+      <c r="P3" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="2" t="s">
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="20" t="s">
+      <c r="V3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20" t="s">
+      <c r="W3" s="23"/>
+      <c r="X3" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="2" t="s">
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AF3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF3" s="29" t="s">
+      <c r="AG3" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21"/>
-      <c r="AK3" s="21"/>
-    </row>
-    <row r="4" spans="1:37" ht="14.25" customHeight="1">
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+    </row>
+    <row r="4" spans="1:38" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
       <c r="K4" s="7" t="s">
         <v>54</v>
       </c>
@@ -1345,482 +1387,507 @@
         <v>63</v>
       </c>
       <c r="T4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="X4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="Y4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AC4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="AE4" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="AF4" s="8" t="s">
         <v>29</v>
       </c>
       <c r="AG4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AH4" s="21"/>
-      <c r="AI4" s="21"/>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="21"/>
-    </row>
-    <row r="5" spans="1:37" ht="15">
+      <c r="AI4" s="20"/>
+      <c r="AJ4" s="20"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+    </row>
+    <row r="5" spans="1:38" ht="15">
       <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH5" s="12" t="s">
+      <c r="AI5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" ht="15">
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" ht="15">
       <c r="B6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH6" s="6" t="s">
+      <c r="AI6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" ht="15">
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="15">
       <c r="C7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH7" s="6" t="s">
+      <c r="AI7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AJ7" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" ht="15">
+      <c r="AK7" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="15">
       <c r="D8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH8" s="13" t="s">
+      <c r="AI8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AI8" s="13"/>
-      <c r="AJ8" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" ht="15">
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="15">
       <c r="E9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH9" s="1" t="s">
+      <c r="AI9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AI9" s="13" t="s">
+      <c r="AJ9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AJ9" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" ht="15">
+      <c r="AK9" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" ht="15">
       <c r="F10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH10" s="1" t="s">
+      <c r="AI10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AI10" s="13" t="s">
+      <c r="AJ10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AJ10" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" ht="15">
+      <c r="AK10" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="15">
       <c r="G11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH11" s="1" t="s">
+      <c r="AI11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AI11" s="13" t="s">
+      <c r="AJ11" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AJ11" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" ht="15">
+      <c r="AK11" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="15">
       <c r="H12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH12" s="13" t="s">
+      <c r="AI12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AI12" s="1" t="s">
+      <c r="AJ12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AJ12" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" ht="15">
+      <c r="AK12" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" ht="15">
       <c r="I13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH13" s="13" t="s">
+      <c r="AI13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AI13" s="1" t="s">
+      <c r="AJ13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AJ13" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" ht="15">
+      <c r="AK13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="15">
       <c r="J14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH14" s="1" t="s">
+      <c r="AI14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AI14" s="13" t="s">
+      <c r="AJ14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="AJ14" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" ht="15">
+      <c r="AK14" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" ht="15">
       <c r="K15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH15" s="1" t="s">
+      <c r="AI15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AI15" s="1" t="s">
+      <c r="AJ15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AJ15" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" ht="15">
+      <c r="AK15" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" ht="15">
       <c r="L16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH16" s="1" t="s">
+      <c r="AI16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AI16" s="14" t="s">
+      <c r="AJ16" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AJ16" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="13:36" ht="15">
+      <c r="AK16" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="13:37" ht="15">
       <c r="M17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH17" s="1" t="s">
+      <c r="AI17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AI17" s="14" t="s">
+      <c r="AJ17" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="AJ17" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="13:36" ht="15">
+      <c r="AK17" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="13:37" ht="15">
       <c r="N18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH18" s="1" t="s">
+      <c r="AI18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AI18" s="14" t="s">
+      <c r="AJ18" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="AJ18" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="13:36" ht="15">
+      <c r="AK18" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="13:37" ht="15">
       <c r="P19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH19" s="1" t="s">
+      <c r="AI19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AI19" s="16" t="s">
+      <c r="AJ19" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="AJ19" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="13:36" ht="15">
+      <c r="AK19" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="13:37" ht="15">
       <c r="Q20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH20" s="1" t="s">
+      <c r="AI20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AI20" s="16"/>
-      <c r="AJ20" s="17"/>
-    </row>
-    <row r="21" spans="13:36" ht="15">
+      <c r="AJ20" s="30"/>
+      <c r="AK20" s="31"/>
+    </row>
+    <row r="21" spans="13:37" ht="15">
       <c r="R21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH21" s="1" t="s">
+      <c r="AI21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AI21" s="16"/>
-      <c r="AJ21" s="17"/>
-    </row>
-    <row r="22" spans="13:36" ht="15">
+      <c r="AJ21" s="30"/>
+      <c r="AK21" s="31"/>
+    </row>
+    <row r="22" spans="13:37" ht="15">
       <c r="S22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AH22" s="1" t="s">
+      <c r="T22" s="19"/>
+      <c r="AI22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI22" s="16"/>
-      <c r="AJ22" s="17"/>
-    </row>
-    <row r="23" spans="13:36" ht="15">
-      <c r="T23" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH23" s="13" t="s">
+      <c r="AJ22" s="30"/>
+      <c r="AK22" s="31"/>
+    </row>
+    <row r="23" spans="13:37" ht="15">
+      <c r="S23" s="19"/>
+      <c r="T23" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI23" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ23" s="16"/>
+      <c r="AK23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="13:37" ht="15">
+      <c r="U24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AI23" s="13"/>
-      <c r="AJ23" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="13:36" ht="15">
-      <c r="U24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH24" s="1" t="s">
+      <c r="AJ24" s="13"/>
+      <c r="AK24" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="13:37" ht="15">
+      <c r="V25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AI24" s="1" t="s">
+      <c r="AJ25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AJ24" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="13:36" ht="15">
-      <c r="V25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH25" s="1" t="s">
+      <c r="AK25" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="13:37" ht="15">
+      <c r="W26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AI25" s="1"/>
-      <c r="AJ25" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="13:36" ht="15">
-      <c r="W26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH26" s="13" t="s">
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="13:37" ht="15">
+      <c r="X27" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI27" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AI26" s="1"/>
-      <c r="AJ26" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="13:36" ht="15">
-      <c r="X27" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH27" s="13" t="s">
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="13:37" ht="15">
+      <c r="Y28" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI28" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AI27" s="13"/>
-      <c r="AJ27" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="13:36" ht="15">
-      <c r="Y28" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH28" s="13" t="s">
+      <c r="AJ28" s="13"/>
+      <c r="AK28" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="13:37" ht="15">
+      <c r="Z29" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI29" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AI28" s="13" t="s">
+      <c r="AJ29" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="AJ28" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="13:36" ht="15">
-      <c r="Z29" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH29" s="1" t="s">
+      <c r="AK29" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="13:37" ht="15">
+      <c r="AA30" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AI29" s="1" t="s">
+      <c r="AJ30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AJ29" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="13:36" ht="15">
-      <c r="AA30" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH30" s="1" t="s">
+      <c r="AK30" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="13:37" ht="15">
+      <c r="AB31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AI30" s="13" t="s">
+      <c r="AJ31" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="AJ30" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="13:36" ht="15">
-      <c r="AB31" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH31" s="1" t="s">
+      <c r="AK31" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="13:37" ht="15">
+      <c r="AC32" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AI31" s="13" t="s">
+      <c r="AJ32" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="AJ31" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="13:36" ht="15">
-      <c r="AC32" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH32" s="1" t="s">
+      <c r="AK32" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="30:37" ht="15">
+      <c r="AD33" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AI32" s="1" t="s">
+      <c r="AJ33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AJ32" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="30:36" ht="15">
-      <c r="AD33" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH33" s="1" t="s">
+      <c r="AK33" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="30:37" ht="15">
+      <c r="AE34" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AI33" s="13" t="s">
+      <c r="AJ34" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="AJ33" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="30:36" ht="15">
-      <c r="AE34" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF34" s="28"/>
-      <c r="AH34" s="1" t="s">
+      <c r="AK34" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="30:37" ht="15">
+      <c r="AF35" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG35" s="19"/>
+      <c r="AI35" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AI34" s="1"/>
-      <c r="AJ34" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="30:36" ht="15">
-      <c r="AE35" s="28"/>
-      <c r="AF35" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH35" s="14" t="s">
+      <c r="AJ35" s="1"/>
+      <c r="AK35" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="30:37" ht="15">
+      <c r="AF36" s="19"/>
+      <c r="AG36" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI36" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AI35" s="14"/>
-      <c r="AJ35" s="15"/>
-    </row>
-    <row r="36" spans="30:36" ht="15">
-      <c r="AG36" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH36" s="1" t="s">
+      <c r="AJ36" s="14"/>
+      <c r="AK36" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="30:37" ht="15">
+      <c r="AH37" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AI36" s="1" t="s">
+      <c r="AJ37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AJ36" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="30:36">
-      <c r="AI37" s="1"/>
+      <c r="AK37" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="30:37">
+      <c r="AJ38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AJ19:AJ22"/>
+    <mergeCell ref="AK19:AK22"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="AJ1:AJ4"/>
     <mergeCell ref="AK1:AK4"/>
-    <mergeCell ref="T1:AG2"/>
-    <mergeCell ref="AH1:AH4"/>
+    <mergeCell ref="AL1:AL4"/>
+    <mergeCell ref="U1:AH2"/>
+    <mergeCell ref="AI1:AI4"/>
     <mergeCell ref="P3:S3"/>
     <mergeCell ref="A1:S2"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:O3"/>
     <mergeCell ref="N4:O4"/>
@@ -1828,13 +1895,7 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AI19:AI22"/>
-    <mergeCell ref="AJ19:AJ22"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="AI1:AI4"/>
-    <mergeCell ref="AJ1:AJ4"/>
+    <mergeCell ref="AG3:AH3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157505" bottom="0.39370078740157505" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>